<commit_message>
Added mouser links for FCU parts
</commit_message>
<xml_diff>
--- a/electrical/parts/compiled_parts.xlsx
+++ b/electrical/parts/compiled_parts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="433">
   <si>
     <t>Designator</t>
   </si>
@@ -1290,6 +1290,30 @@
   </si>
   <si>
     <t>http://www.futureelectronics.com/en/technologies/interconnect/connectors-pcb/socket-plug-board-mount/Pages/8109985-LPPB102NFSP-RC.aspx</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/TXB0108PWR/?qs=sGAEpiMZZMsty6Jaj0%252bBBhonw%2flHfIB47h2ZBZc1b4s%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/MAX3221CPW/?qs=sGAEpiMZZMutXGli8Ay4kGzBZxTNUF2pfDMlx7%252bOkrY%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/UA78M05CDCYR/?qs=sGAEpiMZZMtUqDgmOWBjgDRL0v%252b7sWT8CqGKJibCrHc%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/UA78M33CDCY/?qs=sGAEpiMZZMtUqDgmOWBjgHbKmseNGGTSkgouR6SXN0g%3d</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/54819-0572/?qs=sGAEpiMZZMulM8LPOQ%252bykzAp4yt8IxVboHG1FDrEqZY%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/35363-0460/?qs=%2fThcE39Bh8otk12cQaMDIg%3d%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Molex/35363-0360/?qs=e7FQyhQEwjenRHimJE4bFQ%3d%3d</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1324,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1324,6 +1348,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1422,7 +1454,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1430,8 +1462,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1472,14 +1505,16 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="40% - Accent2" xfId="1" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
     <cellStyle name="40% - Accent4" xfId="3" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
     <cellStyle name="40% - Accent6" xfId="5" builtinId="51"/>
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1779,10 +1814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N124"/>
+  <dimension ref="A1:O124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C81" workbookViewId="0">
-      <selection activeCell="M102" sqref="M102"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>68</v>
       </c>
@@ -2385,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>71</v>
       </c>
@@ -2421,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>77</v>
       </c>
@@ -2457,7 +2492,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>84</v>
       </c>
@@ -2493,13 +2528,13 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>90</v>
       </c>
@@ -2508,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2540,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
@@ -2572,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>92</v>
       </c>
@@ -2608,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>96</v>
       </c>
@@ -2644,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>102</v>
       </c>
@@ -2679,8 +2714,11 @@
       <c r="M27" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>108</v>
       </c>
@@ -2715,8 +2753,11 @@
       <c r="M28" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="36" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>110</v>
       </c>
@@ -2752,7 +2793,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>111</v>
       </c>
@@ -2788,7 +2829,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>113</v>
       </c>
@@ -2823,8 +2864,11 @@
       <c r="M31" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>117</v>
       </c>
@@ -2859,8 +2903,11 @@
       <c r="M32" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="36" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>119</v>
       </c>
@@ -2896,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>124</v>
       </c>
@@ -2932,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>126</v>
       </c>
@@ -2968,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>128</v>
       </c>
@@ -3004,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>130</v>
       </c>
@@ -3039,8 +3086,14 @@
       <c r="M37" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>427</v>
+      </c>
+      <c r="O37" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>133</v>
       </c>
@@ -3076,7 +3129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>136</v>
       </c>
@@ -3112,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>141</v>
       </c>
@@ -3147,8 +3200,11 @@
       <c r="M40" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="36" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>146</v>
       </c>
@@ -3183,8 +3239,11 @@
       <c r="M41" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="36" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>149</v>
       </c>
@@ -3220,13 +3279,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
         <v>398</v>
       </c>
@@ -3235,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -3267,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>152</v>
       </c>
@@ -3303,7 +3362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>155</v>
       </c>
@@ -3339,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>159</v>
       </c>
@@ -5961,8 +6020,15 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N40" r:id="rId1"/>
+    <hyperlink ref="N41" r:id="rId2"/>
+    <hyperlink ref="N27" r:id="rId3"/>
+    <hyperlink ref="N28" r:id="rId4"/>
+    <hyperlink ref="N32" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Parts order mostly done.
</commit_message>
<xml_diff>
--- a/electrical/parts/compiled_parts.xlsx
+++ b/electrical/parts/compiled_parts.xlsx
@@ -1816,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,8 +2711,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M27" s="33">
-        <v>0</v>
+      <c r="M27">
+        <v>1</v>
       </c>
       <c r="N27" s="36" t="s">
         <v>430</v>
@@ -2750,8 +2750,8 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="M28" s="33">
-        <v>0</v>
+      <c r="M28">
+        <v>3</v>
       </c>
       <c r="N28" s="36" t="s">
         <v>431</v>
@@ -2900,8 +2900,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M32" s="33">
-        <v>0</v>
+      <c r="M32">
+        <v>1</v>
       </c>
       <c r="N32" s="36" t="s">
         <v>432</v>
@@ -3083,10 +3083,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M37" s="33">
-        <v>0</v>
-      </c>
-      <c r="N37" t="s">
+      <c r="M37">
+        <v>4</v>
+      </c>
+      <c r="N37" s="36" t="s">
         <v>427</v>
       </c>
       <c r="O37" t="s">
@@ -3197,8 +3197,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M40" s="33">
-        <v>0</v>
+      <c r="M40">
+        <v>1</v>
       </c>
       <c r="N40" s="36" t="s">
         <v>425</v>
@@ -3236,8 +3236,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M41" s="33">
-        <v>0</v>
+      <c r="M41">
+        <v>1</v>
       </c>
       <c r="N41" s="36" t="s">
         <v>426</v>
@@ -6026,9 +6026,10 @@
     <hyperlink ref="N27" r:id="rId3"/>
     <hyperlink ref="N28" r:id="rId4"/>
     <hyperlink ref="N32" r:id="rId5"/>
+    <hyperlink ref="N37" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finished ordering all parts except 20-pin female header for imu.
</commit_message>
<xml_diff>
--- a/electrical/parts/compiled_parts.xlsx
+++ b/electrical/parts/compiled_parts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="435">
   <si>
     <t>Designator</t>
   </si>
@@ -1286,9 +1286,6 @@
     <t>Ordered</t>
   </si>
   <si>
-    <t>out of stock digikey and mouser</t>
-  </si>
-  <si>
     <t>http://www.futureelectronics.com/en/technologies/interconnect/connectors-pcb/socket-plug-board-mount/Pages/8109985-LPPB102NFSP-RC.aspx</t>
   </si>
   <si>
@@ -1314,6 +1311,15 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/Molex/35363-0360/?qs=e7FQyhQEwjenRHimJE4bFQ%3d%3d</t>
+  </si>
+  <si>
+    <t>joey says aaron will give us XMEGAs</t>
+  </si>
+  <si>
+    <t>digi</t>
+  </si>
+  <si>
+    <t>need samples from ti??</t>
   </si>
 </sst>
 </file>
@@ -1814,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O124"/>
+  <dimension ref="A1:Q124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="E102" workbookViewId="0">
+      <selection activeCell="Q128" sqref="Q128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1832,7 +1838,7 @@
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>89</v>
       </c>
@@ -1848,8 +1854,14 @@
       <c r="M1" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1881,7 +1893,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1917,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1953,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1989,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -2025,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -2061,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>33</v>
       </c>
@@ -2097,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -2132,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -2167,8 +2179,11 @@
       <c r="M10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
@@ -2203,8 +2218,11 @@
       <c r="M11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -2240,7 +2258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>55</v>
       </c>
@@ -2276,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>60</v>
       </c>
@@ -2312,7 +2330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
@@ -2348,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>65</v>
       </c>
@@ -2384,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>68</v>
       </c>
@@ -2420,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>71</v>
       </c>
@@ -2452,11 +2470,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M18" s="33">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>77</v>
       </c>
@@ -2485,14 +2506,14 @@
         <v>83</v>
       </c>
       <c r="K19">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>84</v>
       </c>
@@ -2521,20 +2542,20 @@
         <v>12</v>
       </c>
       <c r="K20">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L20">
         <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>90</v>
       </c>
@@ -2543,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2575,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
@@ -2607,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>92</v>
       </c>
@@ -2643,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>96</v>
       </c>
@@ -2679,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>102</v>
       </c>
@@ -2715,10 +2736,13 @@
         <v>1</v>
       </c>
       <c r="N27" s="36" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+      <c r="P27" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>108</v>
       </c>
@@ -2754,10 +2778,13 @@
         <v>3</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+      <c r="P28" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>110</v>
       </c>
@@ -2793,7 +2820,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>111</v>
       </c>
@@ -2829,7 +2856,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>113</v>
       </c>
@@ -2865,10 +2892,10 @@
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>117</v>
       </c>
@@ -2901,13 +2928,16 @@
         <v>1</v>
       </c>
       <c r="M32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N32" s="36" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+      <c r="P32" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>119</v>
       </c>
@@ -2943,7 +2973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>124</v>
       </c>
@@ -2979,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>126</v>
       </c>
@@ -3015,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>128</v>
       </c>
@@ -3051,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>130</v>
       </c>
@@ -3087,13 +3117,16 @@
         <v>4</v>
       </c>
       <c r="N37" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="O37" t="s">
         <v>427</v>
       </c>
-      <c r="O37" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>133</v>
       </c>
@@ -3126,10 +3159,10 @@
         <v>1</v>
       </c>
       <c r="M38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>136</v>
       </c>
@@ -3164,8 +3197,11 @@
       <c r="M39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q39" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>141</v>
       </c>
@@ -3198,13 +3234,16 @@
         <v>1</v>
       </c>
       <c r="M40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N40" s="36" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+      <c r="P40" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>146</v>
       </c>
@@ -3232,18 +3271,21 @@
       <c r="I41" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="K41">
+        <v>5</v>
+      </c>
       <c r="L41">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="M41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41" s="36" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>149</v>
       </c>
@@ -3278,14 +3320,17 @@
       <c r="M42">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q42" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="30" t="s">
         <v>398</v>
       </c>
@@ -3294,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -3326,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>152</v>
       </c>
@@ -3362,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>155</v>
       </c>
@@ -3398,7 +3443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>159</v>
       </c>
@@ -3434,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>39</v>
       </c>
@@ -3469,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>166</v>
       </c>
@@ -3505,7 +3550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>168</v>
       </c>
@@ -3533,24 +3578,21 @@
       <c r="I51" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="K51">
+        <v>6</v>
+      </c>
       <c r="L51">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M51" s="33">
-        <v>0</v>
-      </c>
-      <c r="N51" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>171</v>
       </c>
@@ -3559,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -3591,7 +3633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>172</v>
       </c>
@@ -3626,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>174</v>
       </c>
@@ -3662,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>372</v>
       </c>
@@ -3698,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>179</v>
       </c>
@@ -3734,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>183</v>
       </c>
@@ -3770,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>187</v>
       </c>
@@ -3806,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>191</v>
       </c>
@@ -3842,7 +3884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>195</v>
       </c>
@@ -3878,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>198</v>
       </c>
@@ -3914,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>204</v>
       </c>
@@ -3950,7 +3992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>39</v>
       </c>
@@ -3986,7 +4028,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>43</v>
       </c>
@@ -4019,10 +4061,13 @@
         <v>1</v>
       </c>
       <c r="M66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>47</v>
       </c>
@@ -4057,8 +4102,11 @@
       <c r="M67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q67" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>215</v>
       </c>
@@ -4094,7 +4142,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>221</v>
       </c>
@@ -4130,7 +4178,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>223</v>
       </c>
@@ -4166,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>226</v>
       </c>
@@ -4202,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>230</v>
       </c>
@@ -4238,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>234</v>
       </c>
@@ -4274,7 +4322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>237</v>
       </c>
@@ -4310,7 +4358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>239</v>
       </c>
@@ -4346,7 +4394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>242</v>
       </c>
@@ -4382,7 +4430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>245</v>
       </c>
@@ -4418,7 +4466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>248</v>
       </c>
@@ -4454,7 +4502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>249</v>
       </c>
@@ -4490,7 +4538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>71</v>
       </c>
@@ -4591,11 +4639,11 @@
         <v>83</v>
       </c>
       <c r="K82">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L82">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4631,7 +4679,7 @@
         <v>1</v>
       </c>
       <c r="M83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4993,7 +5041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>285</v>
       </c>
@@ -5029,7 +5077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>291</v>
       </c>
@@ -5065,7 +5113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>296</v>
       </c>
@@ -5101,7 +5149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
         <v>204</v>
       </c>
@@ -5137,7 +5185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
         <v>303</v>
       </c>
@@ -5173,8 +5221,11 @@
       <c r="M101">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q101" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>47</v>
       </c>
@@ -5211,10 +5262,10 @@
         <v>0</v>
       </c>
       <c r="N102" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
         <v>110</v>
       </c>
@@ -5251,7 +5302,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>310</v>
       </c>
@@ -5287,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
         <v>312</v>
       </c>
@@ -5323,7 +5374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
         <v>313</v>
       </c>
@@ -5359,7 +5410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
         <v>314</v>
       </c>
@@ -5395,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
         <v>315</v>
       </c>
@@ -5431,7 +5482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
         <v>318</v>
       </c>
@@ -5467,7 +5518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
         <v>319</v>
       </c>
@@ -5503,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
         <v>322</v>
       </c>
@@ -5538,7 +5589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
         <v>323</v>
       </c>
@@ -5573,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
         <v>325</v>
       </c>
@@ -5608,7 +5659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
         <v>327</v>
       </c>
@@ -5643,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
         <v>328</v>
       </c>
@@ -5679,11 +5730,14 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M115">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M115" s="33">
+        <v>0</v>
+      </c>
+      <c r="N115" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
         <v>168</v>
       </c>
@@ -5720,7 +5774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
         <v>133</v>
       </c>
@@ -5756,8 +5810,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M117">
+        <v>1</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
         <v>136</v>
       </c>
@@ -5793,8 +5853,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M118">
+        <v>1</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
         <v>141</v>
       </c>
@@ -5830,8 +5896,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M119">
+        <v>1</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
         <v>146</v>
       </c>
@@ -5861,14 +5933,14 @@
       </c>
       <c r="J120" s="27"/>
       <c r="K120">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L120">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
         <v>352</v>
       </c>
@@ -5898,17 +5970,14 @@
       </c>
       <c r="J121" s="27"/>
       <c r="K121">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L121">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
         <v>84</v>
       </c>
@@ -5938,14 +6007,14 @@
       </c>
       <c r="J122" s="27"/>
       <c r="K122">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L122">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
         <v>363</v>
       </c>
@@ -5979,10 +6048,13 @@
         <v>1</v>
       </c>
       <c r="M123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
         <v>367</v>
       </c>
@@ -6037,8 +6109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6120,6 +6192,9 @@
         <f t="shared" ref="H2:H41" si="0">E2*G2</f>
         <v>1.716</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="J2">
         <v>250</v>
       </c>
@@ -6171,6 +6246,9 @@
         <f t="shared" si="0"/>
         <v>24.42</v>
       </c>
+      <c r="I3" t="s">
+        <v>433</v>
+      </c>
       <c r="K3">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6212,8 +6290,8 @@
         <f t="shared" si="0"/>
         <v>4.4800000000000004</v>
       </c>
-      <c r="I4" t="s">
-        <v>387</v>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4">
         <v>10</v>
@@ -6345,6 +6423,9 @@
         <f t="shared" si="0"/>
         <v>2.56</v>
       </c>
+      <c r="I7" t="s">
+        <v>433</v>
+      </c>
       <c r="K7">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -6427,6 +6508,9 @@
         <f t="shared" si="0"/>
         <v>0.38400000000000001</v>
       </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
       <c r="J9">
         <v>70</v>
       </c>
@@ -6468,6 +6552,9 @@
         <f t="shared" si="0"/>
         <v>6.82</v>
       </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
       <c r="J10">
         <v>48</v>
       </c>
@@ -6509,6 +6596,9 @@
         <f t="shared" si="0"/>
         <v>0.3528</v>
       </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
       <c r="J11">
         <v>6</v>
       </c>
@@ -6550,6 +6640,9 @@
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
+      <c r="I12" t="s">
+        <v>433</v>
+      </c>
       <c r="J12">
         <v>4</v>
       </c>
@@ -6591,6 +6684,9 @@
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
       <c r="J13">
         <v>7</v>
       </c>
@@ -6635,6 +6731,9 @@
         <f t="shared" si="0"/>
         <v>0.82800000000000007</v>
       </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
       <c r="J14">
         <v>7</v>
       </c>
@@ -6676,6 +6775,9 @@
         <f t="shared" si="0"/>
         <v>0.17699999999999999</v>
       </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
       <c r="J15">
         <v>7</v>
       </c>
@@ -6717,6 +6819,9 @@
         <f t="shared" si="0"/>
         <v>3.52</v>
       </c>
+      <c r="I16" t="s">
+        <v>433</v>
+      </c>
       <c r="J16">
         <v>4</v>
       </c>
@@ -6758,8 +6863,8 @@
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="I17" t="s">
-        <v>387</v>
+      <c r="I17">
+        <v>0</v>
       </c>
       <c r="J17">
         <v>30</v>
@@ -6802,6 +6907,9 @@
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
       <c r="J18">
         <v>11</v>
       </c>
@@ -6871,6 +6979,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
       <c r="K20">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -6912,6 +7023,9 @@
         <f t="shared" si="0"/>
         <v>6.48</v>
       </c>
+      <c r="I21" t="s">
+        <v>433</v>
+      </c>
       <c r="K21">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -6991,6 +7105,9 @@
         <f t="shared" si="0"/>
         <v>1.3800000000000001</v>
       </c>
+      <c r="I23" t="s">
+        <v>433</v>
+      </c>
       <c r="J23">
         <v>2</v>
       </c>
@@ -7035,6 +7152,9 @@
         <f t="shared" si="0"/>
         <v>9.24</v>
       </c>
+      <c r="I24" t="s">
+        <v>433</v>
+      </c>
       <c r="K24">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -7095,6 +7215,9 @@
         <f t="shared" si="0"/>
         <v>29.52</v>
       </c>
+      <c r="I26" t="s">
+        <v>433</v>
+      </c>
       <c r="K26">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -7117,6 +7240,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
       <c r="K27">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7155,6 +7281,9 @@
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
+      <c r="I28" t="s">
+        <v>433</v>
+      </c>
       <c r="K28">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -7193,6 +7322,9 @@
         <f t="shared" si="0"/>
         <v>0.88</v>
       </c>
+      <c r="I29" t="s">
+        <v>433</v>
+      </c>
       <c r="K29">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -7231,6 +7363,9 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
+      <c r="I30" t="s">
+        <v>433</v>
+      </c>
       <c r="J30">
         <v>10</v>
       </c>
@@ -7272,6 +7407,9 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
       <c r="J31">
         <v>68</v>
       </c>
@@ -7313,6 +7451,9 @@
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
       <c r="J32">
         <v>9</v>
       </c>
@@ -7354,6 +7495,9 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
+      <c r="I33" t="s">
+        <v>433</v>
+      </c>
       <c r="J33">
         <v>2</v>
       </c>
@@ -7395,6 +7539,9 @@
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
+      <c r="I34" t="s">
+        <v>433</v>
+      </c>
       <c r="K34">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -7433,6 +7580,9 @@
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
+      <c r="I35" t="s">
+        <v>433</v>
+      </c>
       <c r="K35">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -7471,6 +7621,9 @@
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
       <c r="J36">
         <v>80</v>
       </c>
@@ -7512,6 +7665,9 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
+      <c r="I37" t="s">
+        <v>433</v>
+      </c>
       <c r="J37">
         <v>2</v>
       </c>
@@ -7555,6 +7711,9 @@
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
       <c r="J38">
         <v>100</v>
       </c>
@@ -7596,6 +7755,9 @@
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
       <c r="J39">
         <v>39</v>
       </c>
@@ -7637,6 +7799,9 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
       <c r="J40">
         <v>8</v>
       </c>
@@ -7674,6 +7839,9 @@
       <c r="H41" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>433</v>
       </c>
       <c r="K41">
         <f t="shared" si="1"/>

</xml_diff>